<commit_message>
22-03-2019 : bugfixed : Overtime calculation on Public Holiday and WeekOff
</commit_message>
<xml_diff>
--- a/upload_template/LeaveBalance_Upload.xlsx
+++ b/upload_template/LeaveBalance_Upload.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>CompCode</t>
   </si>
@@ -39,15 +39,6 @@
     <t>CL</t>
   </si>
   <si>
-    <t>SL</t>
-  </si>
-  <si>
-    <t>PL</t>
-  </si>
-  <si>
-    <t>OH</t>
-  </si>
-  <si>
     <t>01</t>
   </si>
   <si>
@@ -57,7 +48,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -409,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,7 +428,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -445,13 +436,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="1">
-        <v>2017</v>
+        <v>2019</v>
       </c>
       <c r="D2" s="1">
         <v>20005890</v>
@@ -461,66 +452,6 @@
       </c>
       <c r="F2" s="1">
         <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1">
-        <v>2017</v>
-      </c>
-      <c r="D3" s="1">
-        <v>20005890</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="1">
-        <v>2017</v>
-      </c>
-      <c r="D4" s="1">
-        <v>20005890</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="1">
-        <v>2017</v>
-      </c>
-      <c r="D5" s="1">
-        <v>20005890</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="1">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>